<commit_message>
updated for changes in model
</commit_message>
<xml_diff>
--- a/Example input/kansas inputs.xlsx
+++ b/Example input/kansas inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BE4387-E7F6-4502-BF7C-B835E9DFF6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A342FAB3-71D0-4045-8A93-EB16C716D039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18768" yWindow="2100" windowWidth="17280" windowHeight="9132" tabRatio="824" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1752" yWindow="3108" windowWidth="17280" windowHeight="9132" tabRatio="824" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="5" r:id="rId1"/>
@@ -2893,7 +2893,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="948" topLeftCell="A34" activePane="bottomLeft"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>